<commit_message>
Add test demonstrating broken translation delete behavior
</commit_message>
<xml_diff>
--- a/corehq/apps/app_manager/tests/data/bulk_app_translation/basic/upload.xlsx
+++ b/corehq/apps/app_manager/tests/data/bulk_app_translation/basic/upload.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modules_and_forms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
   <si>
     <t>Type</t>
   </si>
@@ -110,9 +110,6 @@
     <t>question4</t>
   </si>
   <si>
-    <t>question5</t>
-  </si>
-  <si>
     <t>question7</t>
   </si>
   <si>
@@ -192,16 +189,35 @@
   </si>
   <si>
     <t>question7-label</t>
+  </si>
+  <si>
+    <t>English Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,13 +240,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -579,10 +599,10 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -631,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -647,7 +667,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -658,69 +678,63 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -728,6 +742,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -740,13 +755,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -780,13 +796,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -809,7 +825,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -838,7 +854,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -867,7 +883,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -896,7 +912,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -925,7 +941,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -954,13 +970,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -983,13 +996,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
change bulk-app translation xlsx files for localized media
</commit_message>
<xml_diff>
--- a/corehq/apps/app_manager/tests/data/bulk_app_translation/basic/upload.xlsx
+++ b/corehq/apps/app_manager/tests/data/bulk_app_translation/basic/upload.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Modules_and_forms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
   <si>
     <t>Type</t>
   </si>
@@ -35,12 +35,6 @@
     <t>default_fra</t>
   </si>
   <si>
-    <t>icon_filepath</t>
-  </si>
-  <si>
-    <t>audio_filepath</t>
-  </si>
-  <si>
     <t>unique_id</t>
   </si>
   <si>
@@ -192,13 +186,25 @@
   </si>
   <si>
     <t>English Label</t>
+  </si>
+  <si>
+    <t>icon_filepath_en</t>
+  </si>
+  <si>
+    <t>audio_filepath_en</t>
+  </si>
+  <si>
+    <t>icon_filepath_fra</t>
+  </si>
+  <si>
+    <t>audio_filepath_fra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +228,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,17 +253,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -556,7 +574,7 @@
     <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,71 +588,77 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -664,10 +688,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -678,71 +702,70 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -767,7 +790,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -776,251 +799,251 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>